<commit_message>
Completed overhaul of "Assign_Subbasin_to_POD.R"
</commit_message>
<xml_diff>
--- a/Demand/InputData/RR_Missing_MainStem_GIS_Manual_Assignment.xlsx
+++ b/Demand/InputData/RR_Missing_MainStem_GIS_Manual_Assignment.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aprashar\Documents\Github\DWRAT_DataScraping\Demand\InputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ECCBA5D-D000-49B7-A6FE-1AD1206C1444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{364AE3BA-6AFF-4AFA-BE36-DCFBC8503DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Missing_MainStem_GIS_Manual_Ass" sheetId="1" r:id="rId1"/>
+    <sheet name="Missing_MainStem_GIS" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="152">
   <si>
     <t>OBJECTID</t>
   </si>
@@ -383,6 +396,99 @@
   </si>
   <si>
     <t>R_06_M</t>
+  </si>
+  <si>
+    <t>Basin_ID</t>
+  </si>
+  <si>
+    <t>Basin_Num</t>
+  </si>
+  <si>
+    <t>Grouping</t>
+  </si>
+  <si>
+    <t>A012919A</t>
+  </si>
+  <si>
+    <t>A012919B</t>
+  </si>
+  <si>
+    <t>A016961</t>
+  </si>
+  <si>
+    <t>A013832</t>
+  </si>
+  <si>
+    <t>A013217</t>
+  </si>
+  <si>
+    <t>A015728B</t>
+  </si>
+  <si>
+    <t>A015779</t>
+  </si>
+  <si>
+    <t>A019351</t>
+  </si>
+  <si>
+    <t>A026298A</t>
+  </si>
+  <si>
+    <t>A015736</t>
+  </si>
+  <si>
+    <t>A015737</t>
+  </si>
+  <si>
+    <t>A024929</t>
+  </si>
+  <si>
+    <t>A029070</t>
+  </si>
+  <si>
+    <t>A013393</t>
+  </si>
+  <si>
+    <t>A012510</t>
+  </si>
+  <si>
+    <t>A020491</t>
+  </si>
+  <si>
+    <t>A022667</t>
+  </si>
+  <si>
+    <t>R_03_M</t>
+  </si>
+  <si>
+    <t>R_10</t>
+  </si>
+  <si>
+    <t>R_10_M</t>
+  </si>
+  <si>
+    <t>R_13_M</t>
+  </si>
+  <si>
+    <t>R_14_M</t>
+  </si>
+  <si>
+    <t>R_17</t>
+  </si>
+  <si>
+    <t>R_18_M</t>
+  </si>
+  <si>
+    <t>R_21_M</t>
+  </si>
+  <si>
+    <t>R_23</t>
+  </si>
+  <si>
+    <t>R_24_M</t>
+  </si>
+  <si>
+    <t>R_25</t>
   </si>
 </sst>
 </file>
@@ -401,6 +507,7 @@
       <b/>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -749,13 +856,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AN13"/>
+  <dimension ref="A1:AQ30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:40" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:43" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -876,8 +983,17 @@
       <c r="AN1" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AO1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -986,8 +1102,19 @@
       <c r="AN2">
         <v>-123.054169</v>
       </c>
-    </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AO2" t="str">
+        <f>IF(AQ2 = "Upper", "U_", "L_") &amp; AP2</f>
+        <v>U_6</v>
+      </c>
+      <c r="AP2">
+        <v>6</v>
+      </c>
+      <c r="AQ2" t="str">
+        <f>IF(AP2 &lt; 14, "Upper", "Lower")</f>
+        <v>Upper</v>
+      </c>
+    </row>
+    <row r="3" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1099,8 +1226,19 @@
       <c r="AN3">
         <v>-123.11675099999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AO3" t="str">
+        <f t="shared" ref="AO3:AO30" si="0">IF(AQ3 = "Upper", "U_", "L_") &amp; AP3</f>
+        <v>U_2</v>
+      </c>
+      <c r="AP3">
+        <v>2</v>
+      </c>
+      <c r="AQ3" t="str">
+        <f t="shared" ref="AQ3:AQ30" si="1">IF(AP3 &lt; 14, "Upper", "Lower")</f>
+        <v>Upper</v>
+      </c>
+    </row>
+    <row r="4" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1212,8 +1350,19 @@
       <c r="AN4">
         <v>-122.95836</v>
       </c>
-    </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AO4" t="str">
+        <f t="shared" si="0"/>
+        <v>L_16</v>
+      </c>
+      <c r="AP4">
+        <v>16</v>
+      </c>
+      <c r="AQ4" t="str">
+        <f t="shared" si="1"/>
+        <v>Lower</v>
+      </c>
+    </row>
+    <row r="5" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1319,8 +1468,19 @@
       <c r="AN5">
         <v>-123.192717</v>
       </c>
-    </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AO5" t="str">
+        <f t="shared" si="0"/>
+        <v>U_4</v>
+      </c>
+      <c r="AP5">
+        <v>4</v>
+      </c>
+      <c r="AQ5" t="str">
+        <f t="shared" si="1"/>
+        <v>Upper</v>
+      </c>
+    </row>
+    <row r="6" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1432,8 +1592,19 @@
       <c r="AN6">
         <v>-122.817803</v>
       </c>
-    </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AO6" t="str">
+        <f t="shared" si="0"/>
+        <v>U_12</v>
+      </c>
+      <c r="AP6">
+        <v>12</v>
+      </c>
+      <c r="AQ6" t="str">
+        <f t="shared" si="1"/>
+        <v>Upper</v>
+      </c>
+    </row>
+    <row r="7" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1539,8 +1710,19 @@
       <c r="AN7">
         <v>-122.853348</v>
       </c>
-    </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AO7" t="str">
+        <f t="shared" si="0"/>
+        <v>U_12</v>
+      </c>
+      <c r="AP7">
+        <v>12</v>
+      </c>
+      <c r="AQ7" t="str">
+        <f t="shared" si="1"/>
+        <v>Upper</v>
+      </c>
+    </row>
+    <row r="8" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1631,8 +1813,19 @@
       <c r="AN8">
         <v>-123.129797</v>
       </c>
-    </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AO8" t="str">
+        <f t="shared" si="0"/>
+        <v>U_2</v>
+      </c>
+      <c r="AP8">
+        <v>2</v>
+      </c>
+      <c r="AQ8" t="str">
+        <f t="shared" si="1"/>
+        <v>Upper</v>
+      </c>
+    </row>
+    <row r="9" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1735,8 +1928,19 @@
       <c r="AN9">
         <v>-122.803932</v>
       </c>
-    </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AO9" t="str">
+        <f t="shared" si="0"/>
+        <v>U_12</v>
+      </c>
+      <c r="AP9">
+        <v>12</v>
+      </c>
+      <c r="AQ9" t="str">
+        <f t="shared" si="1"/>
+        <v>Upper</v>
+      </c>
+    </row>
+    <row r="10" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1839,8 +2043,19 @@
       <c r="AN10">
         <v>-123.103854</v>
       </c>
-    </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AO10" t="str">
+        <f t="shared" si="0"/>
+        <v>L_20</v>
+      </c>
+      <c r="AP10">
+        <v>20</v>
+      </c>
+      <c r="AQ10" t="str">
+        <f t="shared" si="1"/>
+        <v>Lower</v>
+      </c>
+    </row>
+    <row r="11" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1934,8 +2149,19 @@
       <c r="AN11">
         <v>-122.965242</v>
       </c>
-    </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AO11" t="str">
+        <f t="shared" si="0"/>
+        <v>U_9</v>
+      </c>
+      <c r="AP11">
+        <v>9</v>
+      </c>
+      <c r="AQ11" t="str">
+        <f t="shared" si="1"/>
+        <v>Upper</v>
+      </c>
+    </row>
+    <row r="12" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2029,8 +2255,19 @@
       <c r="AN12">
         <v>-122.81699999999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AO12" t="str">
+        <f t="shared" si="0"/>
+        <v>U_12</v>
+      </c>
+      <c r="AP12">
+        <v>12</v>
+      </c>
+      <c r="AQ12" t="str">
+        <f t="shared" si="1"/>
+        <v>Upper</v>
+      </c>
+    </row>
+    <row r="13" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2126,6 +2363,391 @@
       </c>
       <c r="AN13">
         <v>-122.89254</v>
+      </c>
+      <c r="AO13" t="str">
+        <f t="shared" si="0"/>
+        <v>L_16</v>
+      </c>
+      <c r="AP13">
+        <v>16</v>
+      </c>
+      <c r="AQ13" t="str">
+        <f t="shared" si="1"/>
+        <v>Lower</v>
+      </c>
+    </row>
+    <row r="14" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>124</v>
+      </c>
+      <c r="AK14" t="s">
+        <v>141</v>
+      </c>
+      <c r="AO14" t="str">
+        <f t="shared" si="0"/>
+        <v>U_3</v>
+      </c>
+      <c r="AP14">
+        <v>3</v>
+      </c>
+      <c r="AQ14" t="str">
+        <f t="shared" si="1"/>
+        <v>Upper</v>
+      </c>
+    </row>
+    <row r="15" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>137</v>
+      </c>
+      <c r="AK15" t="s">
+        <v>150</v>
+      </c>
+      <c r="AO15" t="str">
+        <f t="shared" si="0"/>
+        <v>L_24</v>
+      </c>
+      <c r="AP15">
+        <v>24</v>
+      </c>
+      <c r="AQ15" t="str">
+        <f t="shared" si="1"/>
+        <v>Lower</v>
+      </c>
+    </row>
+    <row r="16" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>133</v>
+      </c>
+      <c r="AK16" t="s">
+        <v>147</v>
+      </c>
+      <c r="AO16" t="str">
+        <f t="shared" si="0"/>
+        <v>L_18</v>
+      </c>
+      <c r="AP16">
+        <v>18</v>
+      </c>
+      <c r="AQ16" t="str">
+        <f t="shared" si="1"/>
+        <v>Lower</v>
+      </c>
+    </row>
+    <row r="17" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>134</v>
+      </c>
+      <c r="AK17" t="s">
+        <v>147</v>
+      </c>
+      <c r="AO17" t="str">
+        <f t="shared" si="0"/>
+        <v>L_18</v>
+      </c>
+      <c r="AP17">
+        <v>18</v>
+      </c>
+      <c r="AQ17" t="str">
+        <f t="shared" si="1"/>
+        <v>Lower</v>
+      </c>
+    </row>
+    <row r="18" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>131</v>
+      </c>
+      <c r="AK18" t="s">
+        <v>145</v>
+      </c>
+      <c r="AO18" t="str">
+        <f t="shared" si="0"/>
+        <v>L_14</v>
+      </c>
+      <c r="AP18">
+        <v>14</v>
+      </c>
+      <c r="AQ18" t="str">
+        <f t="shared" si="1"/>
+        <v>Lower</v>
+      </c>
+    </row>
+    <row r="19" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>132</v>
+      </c>
+      <c r="AK19" t="s">
+        <v>146</v>
+      </c>
+      <c r="AO19" t="str">
+        <f t="shared" si="0"/>
+        <v>L_17</v>
+      </c>
+      <c r="AP19">
+        <v>17</v>
+      </c>
+      <c r="AQ19" t="str">
+        <f t="shared" si="1"/>
+        <v>Lower</v>
+      </c>
+    </row>
+    <row r="20" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>7</v>
+      </c>
+      <c r="B20" t="s">
+        <v>135</v>
+      </c>
+      <c r="AK20" t="s">
+        <v>148</v>
+      </c>
+      <c r="AO20" t="str">
+        <f t="shared" si="0"/>
+        <v>L_21</v>
+      </c>
+      <c r="AP20">
+        <v>21</v>
+      </c>
+      <c r="AQ20" t="str">
+        <f t="shared" si="1"/>
+        <v>Lower</v>
+      </c>
+    </row>
+    <row r="21" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>8</v>
+      </c>
+      <c r="B21" t="s">
+        <v>125</v>
+      </c>
+      <c r="AK21" t="s">
+        <v>141</v>
+      </c>
+      <c r="AO21" t="str">
+        <f t="shared" si="0"/>
+        <v>U_3</v>
+      </c>
+      <c r="AP21">
+        <v>3</v>
+      </c>
+      <c r="AQ21" t="str">
+        <f t="shared" si="1"/>
+        <v>Upper</v>
+      </c>
+    </row>
+    <row r="22" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>9</v>
+      </c>
+      <c r="B22" t="s">
+        <v>127</v>
+      </c>
+      <c r="AK22" t="s">
+        <v>143</v>
+      </c>
+      <c r="AO22" t="str">
+        <f t="shared" si="0"/>
+        <v>U_10</v>
+      </c>
+      <c r="AP22">
+        <v>10</v>
+      </c>
+      <c r="AQ22" t="str">
+        <f t="shared" si="1"/>
+        <v>Upper</v>
+      </c>
+    </row>
+    <row r="23" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>10</v>
+      </c>
+      <c r="B23" t="s">
+        <v>126</v>
+      </c>
+      <c r="AK23" t="s">
+        <v>142</v>
+      </c>
+      <c r="AO23" t="str">
+        <f t="shared" si="0"/>
+        <v>U_10</v>
+      </c>
+      <c r="AP23">
+        <v>10</v>
+      </c>
+      <c r="AQ23" t="str">
+        <f t="shared" si="1"/>
+        <v>Upper</v>
+      </c>
+    </row>
+    <row r="24" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>11</v>
+      </c>
+      <c r="B24" t="s">
+        <v>129</v>
+      </c>
+      <c r="AK24" t="s">
+        <v>87</v>
+      </c>
+      <c r="AO24" t="str">
+        <f t="shared" si="0"/>
+        <v>U_12</v>
+      </c>
+      <c r="AP24">
+        <v>12</v>
+      </c>
+      <c r="AQ24" t="str">
+        <f t="shared" si="1"/>
+        <v>Upper</v>
+      </c>
+    </row>
+    <row r="25" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>12</v>
+      </c>
+      <c r="B25" t="s">
+        <v>128</v>
+      </c>
+      <c r="AK25" t="s">
+        <v>87</v>
+      </c>
+      <c r="AO25" t="str">
+        <f t="shared" si="0"/>
+        <v>U_12</v>
+      </c>
+      <c r="AP25">
+        <v>12</v>
+      </c>
+      <c r="AQ25" t="str">
+        <f t="shared" si="1"/>
+        <v>Upper</v>
+      </c>
+    </row>
+    <row r="26" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>13</v>
+      </c>
+      <c r="B26" t="s">
+        <v>130</v>
+      </c>
+      <c r="AK26" t="s">
+        <v>144</v>
+      </c>
+      <c r="AO26" t="str">
+        <f t="shared" si="0"/>
+        <v>U_13</v>
+      </c>
+      <c r="AP26">
+        <v>13</v>
+      </c>
+      <c r="AQ26" t="str">
+        <f t="shared" si="1"/>
+        <v>Upper</v>
+      </c>
+    </row>
+    <row r="27" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>14</v>
+      </c>
+      <c r="B27" t="s">
+        <v>138</v>
+      </c>
+      <c r="AK27" t="s">
+        <v>151</v>
+      </c>
+      <c r="AO27" t="str">
+        <f t="shared" si="0"/>
+        <v>L_25</v>
+      </c>
+      <c r="AP27">
+        <v>25</v>
+      </c>
+      <c r="AQ27" t="str">
+        <f t="shared" si="1"/>
+        <v>Lower</v>
+      </c>
+    </row>
+    <row r="28" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>15</v>
+      </c>
+      <c r="B28" t="s">
+        <v>139</v>
+      </c>
+      <c r="AK28" t="s">
+        <v>151</v>
+      </c>
+      <c r="AO28" t="str">
+        <f t="shared" si="0"/>
+        <v>L_25</v>
+      </c>
+      <c r="AP28">
+        <v>25</v>
+      </c>
+      <c r="AQ28" t="str">
+        <f t="shared" si="1"/>
+        <v>Lower</v>
+      </c>
+    </row>
+    <row r="29" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>16</v>
+      </c>
+      <c r="B29" t="s">
+        <v>140</v>
+      </c>
+      <c r="AK29" t="s">
+        <v>151</v>
+      </c>
+      <c r="AO29" t="str">
+        <f t="shared" si="0"/>
+        <v>L_25</v>
+      </c>
+      <c r="AP29">
+        <v>25</v>
+      </c>
+      <c r="AQ29" t="str">
+        <f t="shared" si="1"/>
+        <v>Lower</v>
+      </c>
+    </row>
+    <row r="30" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>17</v>
+      </c>
+      <c r="B30" t="s">
+        <v>136</v>
+      </c>
+      <c r="AK30" t="s">
+        <v>149</v>
+      </c>
+      <c r="AO30" t="str">
+        <f t="shared" si="0"/>
+        <v>L_23</v>
+      </c>
+      <c r="AP30">
+        <v>23</v>
+      </c>
+      <c r="AQ30" t="str">
+        <f t="shared" si="1"/>
+        <v>Lower</v>
       </c>
     </row>
   </sheetData>

</xml_diff>